<commit_message>
Idealista 2020 & 2021 data treatment
</commit_message>
<xml_diff>
--- a/temporal_landing/renda familiar 2020.xlsx
+++ b/temporal_landing/renda familiar 2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhengyong Ji\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Zhengyong Ji\Documents\GitHub\MDS-ADSDB-Proj1-JiJonas\temporal_landing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938D95DA-83EB-4597-9B5E-ADBC9738C5A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06171041-0F57-44E3-BDBD-5CFE84AAAEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="1750" windowWidth="11090" windowHeight="8710" xr2:uid="{E1018A7A-359B-4CFD-A896-C78758860A03}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{E1018A7A-359B-4CFD-A896-C78758860A03}"/>
   </bookViews>
   <sheets>
     <sheet name="renda" sheetId="1" r:id="rId1"/>
@@ -477,12 +477,6 @@
     <t>la Nova Esquerra de l'Eixample</t>
   </si>
   <si>
-    <t>el Poble Sec - AEI Parc Montjuïc</t>
-  </si>
-  <si>
-    <t>la Marina del Prat Vermell - AEI Zona Franca</t>
-  </si>
-  <si>
     <t>Sants - Badal</t>
   </si>
   <si>
@@ -535,6 +529,12 @@
   </si>
   <si>
     <t>Sant Marti</t>
+  </si>
+  <si>
+    <t>la Marina del Prat Vermell</t>
+  </si>
+  <si>
+    <t>el Poble Sec</t>
   </si>
 </sst>
 </file>
@@ -586,7 +586,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -598,6 +598,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -914,15 +917,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{953D53C2-8B7F-4B57-9F33-EFAAF808FCBB}">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -942,7 +945,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -962,7 +965,7 @@
     </row>
     <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -982,7 +985,7 @@
     </row>
     <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>11</v>
@@ -1002,7 +1005,7 @@
     </row>
     <row r="5" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>13</v>
@@ -1022,7 +1025,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>16</v>
@@ -1042,7 +1045,7 @@
     </row>
     <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>19</v>
@@ -1062,7 +1065,7 @@
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>147</v>
@@ -1082,7 +1085,7 @@
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>148</v>
@@ -1102,7 +1105,7 @@
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>149</v>
@@ -1122,7 +1125,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>27</v>
@@ -1140,12 +1143,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="C12" s="2">
         <v>16.391999999999999</v>
@@ -1160,12 +1163,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>163</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>151</v>
+        <v>161</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>168</v>
       </c>
       <c r="C13" s="2">
         <v>13.231999999999999</v>
@@ -1182,7 +1185,7 @@
     </row>
     <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>32</v>
@@ -1202,7 +1205,7 @@
     </row>
     <row r="15" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>35</v>
@@ -1222,7 +1225,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>38</v>
@@ -1242,7 +1245,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>41</v>
@@ -1262,10 +1265,10 @@
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C18" s="2">
         <v>18.062999999999999</v>
@@ -1282,7 +1285,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>43</v>
@@ -1302,7 +1305,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>46</v>
@@ -1322,7 +1325,7 @@
     </row>
     <row r="21" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>49</v>
@@ -1342,7 +1345,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>52</v>
@@ -1362,7 +1365,7 @@
     </row>
     <row r="23" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>55</v>
@@ -1382,7 +1385,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>58</v>
@@ -1402,7 +1405,7 @@
     </row>
     <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>61</v>
@@ -1422,10 +1425,10 @@
     </row>
     <row r="26" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C26" s="2">
         <v>47.527000000000001</v>
@@ -1442,10 +1445,10 @@
     </row>
     <row r="27" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C27" s="2">
         <v>36.755000000000003</v>
@@ -1462,7 +1465,7 @@
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>67</v>
@@ -1482,7 +1485,7 @@
     </row>
     <row r="29" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>69</v>
@@ -1502,7 +1505,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>71</v>
@@ -1522,7 +1525,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>72</v>
@@ -1542,7 +1545,7 @@
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>74</v>
@@ -1562,10 +1565,10 @@
     </row>
     <row r="33" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C33" s="2">
         <v>23.132000000000001</v>
@@ -1582,7 +1585,7 @@
     </row>
     <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>78</v>
@@ -1602,7 +1605,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>81</v>
@@ -1622,7 +1625,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>83</v>
@@ -1642,10 +1645,10 @@
     </row>
     <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C37" s="2">
         <v>23.416</v>
@@ -1662,7 +1665,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>85</v>
@@ -1682,7 +1685,7 @@
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>88</v>
@@ -1702,7 +1705,7 @@
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>90</v>
@@ -1722,7 +1725,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>92</v>
@@ -1742,10 +1745,10 @@
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C42" s="2">
         <v>24.367000000000001</v>
@@ -1762,7 +1765,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>94</v>
@@ -1782,7 +1785,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>95</v>
@@ -1802,7 +1805,7 @@
     </row>
     <row r="45" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>97</v>
@@ -1822,7 +1825,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>98</v>
@@ -1842,7 +1845,7 @@
     </row>
     <row r="47" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>99</v>
@@ -1862,7 +1865,7 @@
     </row>
     <row r="48" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>101</v>
@@ -1882,7 +1885,7 @@
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>103</v>
@@ -1902,7 +1905,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>104</v>
@@ -1922,7 +1925,7 @@
     </row>
     <row r="51" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>105</v>
@@ -1942,10 +1945,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C52" s="2">
         <v>13.132</v>
@@ -1962,7 +1965,7 @@
     </row>
     <row r="53" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>108</v>
@@ -1982,7 +1985,7 @@
     </row>
     <row r="54" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>109</v>
@@ -2002,7 +2005,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>111</v>
@@ -2022,7 +2025,7 @@
     </row>
     <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>114</v>
@@ -2042,7 +2045,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>116</v>
@@ -2202,10 +2205,10 @@
     </row>
     <row r="65" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C65" s="2">
         <v>20.184000000000001</v>
@@ -2222,7 +2225,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>129</v>
@@ -2242,7 +2245,7 @@
     </row>
     <row r="67" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>131</v>
@@ -2262,7 +2265,7 @@
     </row>
     <row r="68" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>133</v>
@@ -2282,7 +2285,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>136</v>
@@ -2302,7 +2305,7 @@
     </row>
     <row r="70" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>138</v>
@@ -2322,7 +2325,7 @@
     </row>
     <row r="71" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>141</v>
@@ -2342,7 +2345,7 @@
     </row>
     <row r="72" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>142</v>
@@ -2362,7 +2365,7 @@
     </row>
     <row r="73" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A73" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>143</v>
@@ -2382,7 +2385,7 @@
     </row>
     <row r="74" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A74" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>145</v>

</xml_diff>